<commit_message>
Recreated k-means clusters, re-ran models, created new results figures
</commit_message>
<xml_diff>
--- a/data/modeling_data/cluster_table.xlsx
+++ b/data/modeling_data/cluster_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\modeling_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BB36C-F520-4931-9329-F28B5690331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DF96B-F911-447E-83CA-7A2F83202E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="113">
   <si>
     <t>Biome</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Evergreen</t>
+  </si>
+  <si>
+    <t>Average Sap Flux</t>
   </si>
 </sst>
 </file>
@@ -842,7 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,6 +857,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -901,7 +907,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -946,16 +955,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G1048576" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Site Label" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Biome" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MAP" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MAT" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Functional Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Average Wind Speed" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="K-Means Label" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Site Label" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Biome" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MAP" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MAT" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Functional Type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Average Wind Speed" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="K-Means Label" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{2FB32E4F-1567-4EE9-A43F-B8099C34A382}" name="Average Sap Flux" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,10 +1271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G96"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection sqref="A1:H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1285,8 @@
     <col min="4" max="4" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1300,6 +1311,9 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1322,8 +1336,12 @@
         <v>7.2616666666666596</v>
       </c>
       <c r="G2" s="1">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2191.1762286895901</v>
+      </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1345,8 +1363,12 @@
         <v>6.5758333333333301</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>441.482166697465</v>
+      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1368,8 +1390,12 @@
         <v>2.56</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1373.1554859267301</v>
+      </c>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1391,8 +1417,12 @@
         <v>4.6749999999999998</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>6870.1724468805896</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1414,8 +1444,12 @@
         <v>3.7341666666666602</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1276.3877267063499</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1437,8 +1471,12 @@
         <v>3.7341666666666602</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>746.42732153415204</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1460,8 +1498,12 @@
         <v>3.73</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>162.11525569452701</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1483,8 +1525,12 @@
         <v>2.5924999999999998</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>202.12114415026099</v>
+      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1506,8 +1552,12 @@
         <v>2.8958333333333299</v>
       </c>
       <c r="G10" s="1">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3032.57547446028</v>
+      </c>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1531,6 +1581,10 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
+      <c r="H11" s="5">
+        <v>546.98555774142596</v>
+      </c>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1552,8 +1606,12 @@
         <v>3.8925000000000001</v>
       </c>
       <c r="G12" s="1">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>257.74561964580801</v>
+      </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1575,8 +1633,12 @@
         <v>3.2066666666666599</v>
       </c>
       <c r="G13" s="1">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3487.8924831802301</v>
+      </c>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1598,8 +1660,12 @@
         <v>3.5525000000000002</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>718.55463476049295</v>
+      </c>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1621,8 +1687,12 @@
         <v>3.8441666666666601</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3898.7377448264701</v>
+      </c>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1644,10 +1714,14 @@
         <v>3.5916666666666601</v>
       </c>
       <c r="G16" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>2158.2470563347201</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1667,10 +1741,14 @@
         <v>3.5916666666666601</v>
       </c>
       <c r="G17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>670.13430194998705</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1690,10 +1768,14 @@
         <v>3.5916666666666601</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1061.1042953204301</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1713,10 +1795,14 @@
         <v>3.5916666666666601</v>
       </c>
       <c r="G19" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>468.69583764808198</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1736,10 +1822,14 @@
         <v>3.7850000000000001</v>
       </c>
       <c r="G20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>2312.5895015272899</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
@@ -1759,10 +1849,14 @@
         <v>3.7850000000000001</v>
       </c>
       <c r="G21" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H21" s="5">
+        <v>3094.5173315741299</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1782,10 +1876,14 @@
         <v>2.7075</v>
       </c>
       <c r="G22" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>737.57575052675497</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1805,10 +1903,14 @@
         <v>2.7291666666666599</v>
       </c>
       <c r="G23" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1015.50571468268</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -1828,10 +1930,14 @@
         <v>2.7466666666666599</v>
       </c>
       <c r="G24" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>890.45943212825398</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1851,10 +1957,14 @@
         <v>2.9933333333333301</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>498.72280288561501</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1874,10 +1984,14 @@
         <v>2.8849999999999998</v>
       </c>
       <c r="G26" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>165.13329988803301</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1897,10 +2011,14 @@
         <v>2.8849999999999998</v>
       </c>
       <c r="G27" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>114.538888457797</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -1920,10 +2038,14 @@
         <v>2.8849999999999998</v>
       </c>
       <c r="G28" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>225.29789763629901</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -1943,10 +2065,14 @@
         <v>2.8849999999999998</v>
       </c>
       <c r="G29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <v>133.19079573081299</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1966,10 +2092,14 @@
         <v>3.60083333333333</v>
       </c>
       <c r="G30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>240.59421171015401</v>
+      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1989,10 +2119,14 @@
         <v>3.60083333333333</v>
       </c>
       <c r="G31" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>101.46508932514099</v>
+      </c>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -2012,10 +2146,14 @@
         <v>3.60083333333333</v>
       </c>
       <c r="G32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5">
+        <v>353.72029617096399</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2035,10 +2173,14 @@
         <v>4.6524999999999999</v>
       </c>
       <c r="G33" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>404.75173246557603</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -2058,10 +2200,14 @@
         <v>2.4616666666666598</v>
       </c>
       <c r="G34" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>31.016225100101501</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -2081,10 +2227,14 @@
         <v>3.27</v>
       </c>
       <c r="G35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>408.88942213206298</v>
+      </c>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -2104,10 +2254,14 @@
         <v>3.27</v>
       </c>
       <c r="G36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>659.55216504572797</v>
+      </c>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -2127,10 +2281,14 @@
         <v>4.37083333333333</v>
       </c>
       <c r="G37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>92.285289985023596</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -2150,10 +2308,14 @@
         <v>4.3558333333333303</v>
       </c>
       <c r="G38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H38" s="5">
+        <v>153.76444625656501</v>
+      </c>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -2173,10 +2335,14 @@
         <v>4.59</v>
       </c>
       <c r="G39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>696.24132448673004</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -2196,10 +2362,14 @@
         <v>4.59</v>
       </c>
       <c r="G40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>438.70138452759699</v>
+      </c>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -2221,8 +2391,12 @@
       <c r="G41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="5">
+        <v>675.97993923904903</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -2242,10 +2416,14 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="G42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H42" s="5">
+        <v>2319.3539126328801</v>
+      </c>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -2267,8 +2445,12 @@
       <c r="G43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="5">
+        <v>1467.46272020627</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -2288,10 +2470,14 @@
         <v>2.1358333333333301</v>
       </c>
       <c r="G44" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>4658.0795452157799</v>
+      </c>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2311,10 +2497,14 @@
         <v>2.2075</v>
       </c>
       <c r="G45" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>3917.1629285180702</v>
+      </c>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2334,10 +2524,14 @@
         <v>1.29833333333333</v>
       </c>
       <c r="G46" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>3345.8714046366599</v>
+      </c>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2357,10 +2551,14 @@
         <v>1.29</v>
       </c>
       <c r="G47" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1318.65158205183</v>
+      </c>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -2380,10 +2578,14 @@
         <v>2.9008333333333298</v>
       </c>
       <c r="G48" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>944.46302838966506</v>
+      </c>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -2403,10 +2605,14 @@
         <v>2.2741666666666598</v>
       </c>
       <c r="G49" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H49" s="5">
+        <v>860.96052426244796</v>
+      </c>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
@@ -2426,10 +2632,14 @@
         <v>2.2741666666666598</v>
       </c>
       <c r="G50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1084.6132692362701</v>
+      </c>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -2449,10 +2659,14 @@
         <v>3.3616666666666601</v>
       </c>
       <c r="G51" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1120.86049615103</v>
+      </c>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -2472,10 +2686,14 @@
         <v>1.8341666666666601</v>
       </c>
       <c r="G52" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H52" s="5">
+        <v>590.04989877942705</v>
+      </c>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -2495,10 +2713,14 @@
         <v>3.1891666666666598</v>
       </c>
       <c r="G53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5">
+        <v>560.025359663264</v>
+      </c>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -2518,10 +2740,14 @@
         <v>2.7891666666666599</v>
       </c>
       <c r="G54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <v>323.27935884597503</v>
+      </c>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -2541,10 +2767,14 @@
         <v>4.0149999999999997</v>
       </c>
       <c r="G55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <v>492.55672333974502</v>
+      </c>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -2564,10 +2794,14 @@
         <v>4.87083333333333</v>
       </c>
       <c r="G56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H56" s="5">
+        <v>3015.85503909719</v>
+      </c>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
@@ -2587,10 +2821,14 @@
         <v>3.3841666666666601</v>
       </c>
       <c r="G57" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H57" s="5">
+        <v>10042.963389057501</v>
+      </c>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -2610,10 +2848,14 @@
         <v>2.51583333333333</v>
       </c>
       <c r="G58" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5">
+        <v>451.151329050713</v>
+      </c>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>69</v>
       </c>
@@ -2633,10 +2875,14 @@
         <v>2.9241666666666601</v>
       </c>
       <c r="G59" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>1457.8289001748501</v>
+      </c>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -2656,10 +2902,14 @@
         <v>2.9241666666666601</v>
       </c>
       <c r="G60" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1157.22047247965</v>
+      </c>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -2679,10 +2929,14 @@
         <v>2.9241666666666601</v>
       </c>
       <c r="G61" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1020.48850192193</v>
+      </c>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -2702,10 +2956,14 @@
         <v>2.8824999999999998</v>
       </c>
       <c r="G62" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H62" s="5">
+        <v>576.42879212846401</v>
+      </c>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -2725,10 +2983,14 @@
         <v>2.8824999999999998</v>
       </c>
       <c r="G63" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H63" s="5">
+        <v>391.58329802988402</v>
+      </c>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -2748,10 +3010,14 @@
         <v>2.8824999999999998</v>
       </c>
       <c r="G64" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H64" s="5">
+        <v>483.56974235919603</v>
+      </c>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -2771,10 +3037,14 @@
         <v>2.8816666666666602</v>
       </c>
       <c r="G65" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5">
+        <v>730.24131608787798</v>
+      </c>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -2794,10 +3064,14 @@
         <v>2.8816666666666602</v>
       </c>
       <c r="G66" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H66" s="5">
+        <v>475.80257860945198</v>
+      </c>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>77</v>
       </c>
@@ -2817,10 +3091,14 @@
         <v>2.8816666666666602</v>
       </c>
       <c r="G67" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H67" s="5">
+        <v>597.74166085744002</v>
+      </c>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -2842,8 +3120,12 @@
       <c r="G68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="5">
+        <v>634.11764597418801</v>
+      </c>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>79</v>
       </c>
@@ -2863,10 +3145,14 @@
         <v>2.41333333333333</v>
       </c>
       <c r="G69" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H69" s="5">
+        <v>2004.6973591977601</v>
+      </c>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>80</v>
       </c>
@@ -2888,8 +3174,12 @@
       <c r="G70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="5">
+        <v>1290.45307148797</v>
+      </c>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>81</v>
       </c>
@@ -2911,8 +3201,12 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="5">
+        <v>955.13198565647201</v>
+      </c>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -2932,10 +3226,14 @@
         <v>2.4416666666666602</v>
       </c>
       <c r="G72" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H72" s="5">
+        <v>2566.0854674812699</v>
+      </c>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>83</v>
       </c>
@@ -2955,10 +3253,14 @@
         <v>3.59916666666666</v>
       </c>
       <c r="G73" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H73" s="5">
+        <v>1238.09460131384</v>
+      </c>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -2978,10 +3280,14 @@
         <v>3.6733333333333298</v>
       </c>
       <c r="G74" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H74" s="5">
+        <v>2826.7113860243198</v>
+      </c>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>85</v>
       </c>
@@ -3003,8 +3309,12 @@
       <c r="G75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="5">
+        <v>436.24141014030801</v>
+      </c>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
@@ -3026,8 +3336,12 @@
       <c r="G76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="5">
+        <v>501.00477738852197</v>
+      </c>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>87</v>
       </c>
@@ -3049,8 +3363,12 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="5">
+        <v>464.31756357160498</v>
+      </c>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>88</v>
       </c>
@@ -3072,8 +3390,12 @@
       <c r="G78" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="5">
+        <v>396.52127637802801</v>
+      </c>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>89</v>
       </c>
@@ -3095,8 +3417,12 @@
       <c r="G79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="5">
+        <v>1213.1046456306201</v>
+      </c>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>90</v>
       </c>
@@ -3116,10 +3442,14 @@
         <v>3.9258333333333302</v>
       </c>
       <c r="G80" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H80" s="5">
+        <v>178.88013187225499</v>
+      </c>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>92</v>
       </c>
@@ -3139,10 +3469,14 @@
         <v>3.9258333333333302</v>
       </c>
       <c r="G81" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H81" s="5">
+        <v>287.02650977271202</v>
+      </c>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>93</v>
       </c>
@@ -3162,10 +3496,14 @@
         <v>3.9258333333333302</v>
       </c>
       <c r="G82" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H82" s="5">
+        <v>240.599746012396</v>
+      </c>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>94</v>
       </c>
@@ -3187,8 +3525,12 @@
       <c r="G83" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="5">
+        <v>858.64968310095003</v>
+      </c>
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>95</v>
       </c>
@@ -3210,8 +3552,12 @@
       <c r="G84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="5">
+        <v>13.0746209577946</v>
+      </c>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>96</v>
       </c>
@@ -3231,10 +3577,14 @@
         <v>3.5816666666666599</v>
       </c>
       <c r="G85" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H85" s="5">
+        <v>427.25694368310099</v>
+      </c>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>97</v>
       </c>
@@ -3254,10 +3604,14 @@
         <v>2.3616666666666601</v>
       </c>
       <c r="G86" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H86" s="5">
+        <v>1963.5844291009601</v>
+      </c>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>98</v>
       </c>
@@ -3277,10 +3631,14 @@
         <v>1.9824999999999999</v>
       </c>
       <c r="G87" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H87" s="5">
+        <v>1871.26070372447</v>
+      </c>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>99</v>
       </c>
@@ -3302,8 +3660,12 @@
       <c r="G88" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="5">
+        <v>1012.04306631803</v>
+      </c>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>100</v>
       </c>
@@ -3323,10 +3685,14 @@
         <v>2.3883333333333301</v>
       </c>
       <c r="G89" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H89" s="5">
+        <v>2918.9779701928901</v>
+      </c>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>101</v>
       </c>
@@ -3346,10 +3712,14 @@
         <v>3.6383333333333301</v>
       </c>
       <c r="G90" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H90" s="5">
+        <v>1056.0621181000599</v>
+      </c>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>102</v>
       </c>
@@ -3369,10 +3739,14 @@
         <v>3.6225000000000001</v>
       </c>
       <c r="G91" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H91" s="5">
+        <v>967.84125589671305</v>
+      </c>
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>103</v>
       </c>
@@ -3392,10 +3766,14 @@
         <v>3.2083333333333299</v>
       </c>
       <c r="G92" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H92" s="5">
+        <v>3674.93947899762</v>
+      </c>
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>104</v>
       </c>
@@ -3417,8 +3795,12 @@
       <c r="G93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="5">
+        <v>679.63413658368802</v>
+      </c>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>105</v>
       </c>
@@ -3438,10 +3820,14 @@
         <v>3.7941666666666598</v>
       </c>
       <c r="G94" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="5">
+        <v>408.639561818549</v>
+      </c>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>106</v>
       </c>
@@ -3461,10 +3847,14 @@
         <v>3.19</v>
       </c>
       <c r="G95" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H95" s="5">
+        <v>355.748002075675</v>
+      </c>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>107</v>
       </c>
@@ -3484,12 +3874,67 @@
         <v>4.0558333333333296</v>
       </c>
       <c r="G96" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H96" s="5">
+        <v>682.05798989633695</v>
+      </c>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I113" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>